<commit_message>
Slide to the read_exl function regarding dataframe headings due to new file path
</commit_message>
<xml_diff>
--- a/data/Comparison_IRR/001.xlsx
+++ b/data/Comparison_IRR/001.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://w1maccs.sharepoint.com/sites/SLRforABM/Freigegebene Dokumente/General/Analysis/R-code_git_project/SLR_ABMs_Ecology/data/Comparison_IRR/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://w1maccs.sharepoint.com/sites/SLRforABM/Freigegebene Dokumente/General/Content-analysis/ecology_coding_merge/Comparison_IRR/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{1521E97F-D2FB-4859-BEB9-FBBFFDB4538E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{007C91AD-B8E7-455A-9BFA-7048C79586E6}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{1521E97F-D2FB-4859-BEB9-FBBFFDB4538E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0ECCBCA9-C4EE-413A-B87F-CC95A3336C49}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2052,14 +2052,6 @@
     <xf numFmtId="0" fontId="23" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2090,6 +2082,14 @@
     <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2500,17 +2500,17 @@
       <c r="J6" s="2"/>
     </row>
     <row r="10" spans="2:13" ht="14.4">
-      <c r="B10" s="139" t="s">
+      <c r="B10" s="135" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="140"/>
-      <c r="D10" s="140"/>
-      <c r="E10" s="140"/>
-      <c r="F10" s="140"/>
-      <c r="G10" s="140"/>
-      <c r="H10" s="140"/>
-      <c r="I10" s="140"/>
-      <c r="J10" s="141"/>
+      <c r="C10" s="136"/>
+      <c r="D10" s="136"/>
+      <c r="E10" s="136"/>
+      <c r="F10" s="136"/>
+      <c r="G10" s="136"/>
+      <c r="H10" s="136"/>
+      <c r="I10" s="136"/>
+      <c r="J10" s="137"/>
       <c r="K10" s="4"/>
       <c r="L10" s="4"/>
       <c r="M10" s="4"/>
@@ -3725,34 +3725,34 @@
       <c r="F2" s="106" t="s">
         <v>197</v>
       </c>
-      <c r="H2" s="148" t="s">
+      <c r="H2" s="144" t="s">
         <v>169</v>
       </c>
-      <c r="I2" s="148"/>
-      <c r="J2" s="148"/>
-      <c r="L2" s="144" t="s">
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
+      <c r="L2" s="140" t="s">
         <v>198</v>
       </c>
-      <c r="M2" s="145"/>
+      <c r="M2" s="141"/>
     </row>
     <row r="3" spans="2:14" ht="14.4">
       <c r="C3" s="6"/>
       <c r="F3" s="7"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="L3" s="144" t="s">
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="L3" s="140" t="s">
         <v>199</v>
       </c>
-      <c r="M3" s="145"/>
+      <c r="M3" s="141"/>
     </row>
     <row r="4" spans="2:14" ht="30.75" customHeight="1">
       <c r="C4" s="6"/>
       <c r="F4" s="7"/>
-      <c r="L4" s="146" t="s">
+      <c r="L4" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="147"/>
+      <c r="M4" s="143"/>
     </row>
     <row r="5" spans="2:14" thickBot="1">
       <c r="C5" s="8" t="s">
@@ -5656,7 +5656,7 @@
       <c r="H77" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="I77" s="142" t="s">
+      <c r="I77" s="138" t="s">
         <v>158</v>
       </c>
       <c r="L77" s="38" t="s">
@@ -5680,7 +5680,7 @@
       <c r="H78" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="I78" s="143"/>
+      <c r="I78" s="139"/>
       <c r="L78" s="38" t="s">
         <v>6</v>
       </c>
@@ -5702,7 +5702,7 @@
       <c r="H79" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="I79" s="143"/>
+      <c r="I79" s="139"/>
       <c r="L79" s="38" t="s">
         <v>10</v>
       </c>
@@ -9984,8 +9984,8 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="B1:S1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="O90" sqref="O90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" outlineLevelCol="1"/>
@@ -10017,46 +10017,46 @@
       <c r="F2" s="106" t="s">
         <v>197</v>
       </c>
-      <c r="H2" s="148" t="s">
+      <c r="H2" s="144" t="s">
         <v>169</v>
       </c>
-      <c r="I2" s="148"/>
-      <c r="J2" s="148"/>
-      <c r="L2" s="144" t="s">
+      <c r="I2" s="144"/>
+      <c r="J2" s="144"/>
+      <c r="L2" s="140" t="s">
         <v>198</v>
       </c>
-      <c r="M2" s="145"/>
-      <c r="O2" s="149" t="s">
+      <c r="M2" s="141"/>
+      <c r="O2" s="145" t="s">
         <v>210</v>
       </c>
-      <c r="P2" s="150"/>
+      <c r="P2" s="146"/>
     </row>
     <row r="3" spans="2:19">
       <c r="C3" s="6"/>
       <c r="F3" s="7"/>
-      <c r="H3" s="148"/>
-      <c r="I3" s="148"/>
-      <c r="J3" s="148"/>
-      <c r="L3" s="144" t="s">
+      <c r="H3" s="144"/>
+      <c r="I3" s="144"/>
+      <c r="J3" s="144"/>
+      <c r="L3" s="140" t="s">
         <v>199</v>
       </c>
-      <c r="M3" s="145"/>
-      <c r="O3" s="149" t="s">
+      <c r="M3" s="141"/>
+      <c r="O3" s="145" t="s">
         <v>211</v>
       </c>
-      <c r="P3" s="150"/>
+      <c r="P3" s="146"/>
     </row>
     <row r="4" spans="2:19">
       <c r="C4" s="6"/>
       <c r="F4" s="7"/>
-      <c r="L4" s="146" t="s">
+      <c r="L4" s="142" t="s">
         <v>31</v>
       </c>
-      <c r="M4" s="147"/>
-      <c r="O4" s="151" t="s">
+      <c r="M4" s="143"/>
+      <c r="O4" s="147" t="s">
         <v>212</v>
       </c>
-      <c r="P4" s="150"/>
+      <c r="P4" s="146"/>
     </row>
     <row r="5" spans="2:19" ht="15" thickBot="1">
       <c r="C5" s="8" t="s">
@@ -10949,11 +10949,11 @@
       <c r="I33" s="54"/>
       <c r="J33" s="24"/>
       <c r="K33" s="24"/>
-      <c r="L33" s="135" t="s">
+      <c r="L33" s="148" t="s">
         <v>10</v>
       </c>
       <c r="M33" s="28"/>
-      <c r="O33" s="136" t="s">
+      <c r="O33" s="149" t="s">
         <v>6</v>
       </c>
       <c r="P33" s="120"/>
@@ -11566,11 +11566,11 @@
         <v>43</v>
       </c>
       <c r="K49" s="29"/>
-      <c r="L49" s="137" t="s">
+      <c r="L49" s="150" t="s">
         <v>6</v>
       </c>
       <c r="M49" s="35"/>
-      <c r="O49" s="138" t="s">
+      <c r="O49" s="151" t="s">
         <v>6</v>
       </c>
       <c r="P49" s="122"/>
@@ -12459,7 +12459,7 @@
       <c r="H77" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="I77" s="142" t="s">
+      <c r="I77" s="138" t="s">
         <v>158</v>
       </c>
       <c r="L77" s="38" t="s">
@@ -12492,7 +12492,7 @@
       <c r="H78" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="I78" s="143"/>
+      <c r="I78" s="139"/>
       <c r="L78" s="38" t="s">
         <v>6</v>
       </c>
@@ -12523,7 +12523,7 @@
       <c r="H79" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="I79" s="143"/>
+      <c r="I79" s="139"/>
       <c r="L79" s="38" t="s">
         <v>10</v>
       </c>
@@ -12600,11 +12600,11 @@
         <v>43</v>
       </c>
       <c r="K81" s="24"/>
-      <c r="L81" s="137" t="s">
+      <c r="L81" s="150" t="s">
         <v>10</v>
       </c>
       <c r="M81" s="28"/>
-      <c r="O81" s="136" t="s">
+      <c r="O81" s="149" t="s">
         <v>10</v>
       </c>
       <c r="P81" s="120"/>
@@ -12890,11 +12890,11 @@
         <v>43</v>
       </c>
       <c r="K89" s="24"/>
-      <c r="L89" s="135" t="s">
+      <c r="L89" s="148" t="s">
         <v>6</v>
       </c>
       <c r="M89" s="28"/>
-      <c r="O89" s="136" t="s">
+      <c r="O89" s="149" t="s">
         <v>6</v>
       </c>
       <c r="P89" s="120"/>
@@ -16848,7 +16848,6 @@
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="I77:I79"/>
     <mergeCell ref="O2:P2"/>
     <mergeCell ref="O3:P3"/>
     <mergeCell ref="O4:P4"/>
@@ -16856,6 +16855,7 @@
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="L3:M3"/>
     <mergeCell ref="L4:M4"/>
+    <mergeCell ref="I77:I79"/>
   </mergeCells>
   <conditionalFormatting sqref="R1:R1048576">
     <cfRule type="expression" dxfId="1" priority="2">
@@ -16955,14 +16955,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dc8ea9bb-7be6-4347-bbbd-43ecd0226ab6">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="36965efa-5a39-45c9-9312-a4f852bee1e3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -17191,21 +17189,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="dc8ea9bb-7be6-4347-bbbd-43ecd0226ab6">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="36965efa-5a39-45c9-9312-a4f852bee1e3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072C8801-02D8-41B4-9C3A-C0871C6DF7B0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{118A9060-EF27-4670-A7BD-5FE79C142D77}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dc8ea9bb-7be6-4347-bbbd-43ecd0226ab6"/>
-    <ds:schemaRef ds:uri="36965efa-5a39-45c9-9312-a4f852bee1e3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -17230,9 +17227,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{118A9060-EF27-4670-A7BD-5FE79C142D77}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{072C8801-02D8-41B4-9C3A-C0871C6DF7B0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dc8ea9bb-7be6-4347-bbbd-43ecd0226ab6"/>
+    <ds:schemaRef ds:uri="36965efa-5a39-45c9-9312-a4f852bee1e3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>